<commit_message>
This is the load script for the peak annotations and edited test files.
Note that the format detection was implemented before what was implemented in parallel in main.  The version in this PR is flexible in that it doesn't require all sheets or all headers.  It's not a perfect implementation, but it currently works just as well.  It could be made to be better by trying to use optional columns/sheets to identify format.

Files checked in: DataRepo/data/tests/accucor_with_multiple_labels/accucor.xlsx DataRepo/data/tests/accucor_with_multiple_labels/accucor_invalid_label.xlsx DataRepo/data/tests/small_obob/small_obob_maven_6eaas_inf_blank_sample.xlsx DataRepo/data/tests/small_obob/small_obob_maven_6eaas_inf_glucose.xlsx DataRepo/data/tests/small_obob/small_obob_maven_6eaas_inf_glucose_conflicting.xlsx DataRepo/management/commands/load_peak_annotations.py DataRepo/tests/management/test_load_peak_annotations.py
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/accucor_with_multiple_labels/accucor.xlsx
+++ b/DataRepo/data/tests/accucor_with_multiple_labels/accucor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Experiments\Alb ko mice Fcirc\20220818_albKO_mix1_glycerol_150min_infusion_plasma_tail blood\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/data/tests/accucor_with_multiple_labels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4D4D02-C7D7-4057-BE29-1682D674778B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5704C6-7D41-C94F-BAAB-E64B13FD9B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="33">
   <si>
     <t>label</t>
   </si>
@@ -200,9 +200,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -240,9 +240,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,26 +275,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -327,26 +310,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -524,9 +490,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,7 +551,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>3</v>
       </c>
@@ -641,7 +607,7 @@
         <v>76691.199999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>3</v>
       </c>
@@ -694,7 +660,7 @@
         <v>26229.16</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>5</v>
       </c>
@@ -750,7 +716,7 @@
         <v>4330754.5599999996</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>5</v>
       </c>
@@ -803,7 +769,7 @@
         <v>405881.59</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>5</v>
       </c>
@@ -856,7 +822,7 @@
         <v>106599.14</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>5</v>
       </c>
@@ -909,7 +875,7 @@
         <v>515244.34</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>5</v>
       </c>
@@ -962,7 +928,7 @@
         <v>26821.85</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>5</v>
       </c>
@@ -1015,7 +981,7 @@
         <v>7414.33</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>5</v>
       </c>
@@ -1075,13 +1041,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1089,22 +1055,19 @@
         <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1112,22 +1075,19 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1.0402275689662961</v>
+        <v>85750.89959084439</v>
       </c>
       <c r="D2">
-        <v>85750.89959084439</v>
+        <v>113767.0574420943</v>
       </c>
       <c r="E2">
-        <v>113767.0574420943</v>
+        <v>84190.488562416678</v>
       </c>
       <c r="F2">
-        <v>84190.488562416678</v>
-      </c>
-      <c r="G2">
         <v>79775.721893427981</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1146,11 +1106,8 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1169,11 +1126,8 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1187,16 +1141,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>19425.606829438329</v>
       </c>
       <c r="F5">
-        <v>19425.606829438329</v>
-      </c>
-      <c r="G5">
         <v>27219.670232964221</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1204,22 +1155,19 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>1.0789810849249819</v>
+        <v>5591786.8355261376</v>
       </c>
       <c r="D6">
-        <v>5591786.8355261376</v>
+        <v>4910135.5859680166</v>
       </c>
       <c r="E6">
-        <v>4910135.5859680166</v>
+        <v>4380090.4658212066</v>
       </c>
       <c r="F6">
-        <v>4380090.4658212066</v>
-      </c>
-      <c r="G6">
         <v>4692672.7282388248</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1227,22 +1175,19 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>195595.3956708484</v>
       </c>
       <c r="D7">
-        <v>195595.3956708484</v>
+        <v>229303.59604486561</v>
       </c>
       <c r="E7">
-        <v>229303.59604486561</v>
+        <v>138481.27457236411</v>
       </c>
       <c r="F7">
-        <v>138481.27457236411</v>
-      </c>
-      <c r="G7">
         <v>122669.1299826532</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1250,22 +1195,19 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>112278.4380717509</v>
       </c>
       <c r="D8">
-        <v>112278.4380717509</v>
+        <v>154169.69247568949</v>
       </c>
       <c r="E8">
-        <v>154169.69247568949</v>
+        <v>83200.539628753497</v>
       </c>
       <c r="F8">
-        <v>83200.539628753497</v>
-      </c>
-      <c r="G8">
         <v>82870.740571524482</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1273,22 +1215,19 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>137433.18004431319</v>
       </c>
       <c r="D9">
-        <v>137433.18004431319</v>
+        <v>197000.5904698009</v>
       </c>
       <c r="E9">
-        <v>197000.5904698009</v>
+        <v>590367.37452902028</v>
       </c>
       <c r="F9">
-        <v>590367.37452902028</v>
-      </c>
-      <c r="G9">
         <v>551869.74742725445</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1296,22 +1235,19 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>12741.57163112608</v>
       </c>
       <c r="D10">
-        <v>12741.57163112608</v>
+        <v>22989.486835416861</v>
       </c>
       <c r="E10">
-        <v>22989.486835416861</v>
+        <v>5529.4783128642057</v>
       </c>
       <c r="F10">
-        <v>5529.4783128642057</v>
-      </c>
-      <c r="G10">
         <v>9390.2832529520238</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1319,22 +1255,19 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2688.0625616373491</v>
       </c>
       <c r="D11">
-        <v>2688.0625616373491</v>
+        <v>12430.02116063707</v>
       </c>
       <c r="E11">
-        <v>12430.02116063707</v>
+        <v>6595.5721957555343</v>
       </c>
       <c r="F11">
-        <v>6595.5721957555343</v>
-      </c>
-      <c r="G11">
         <v>5684.2671061387146</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1342,18 +1275,15 @@
         <v>6</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>800781.82886352425</v>
       </c>
       <c r="D12">
-        <v>800781.82886352425</v>
+        <v>1155697.9116251131</v>
       </c>
       <c r="E12">
-        <v>1155697.9116251131</v>
+        <v>31197.40939018871</v>
       </c>
       <c r="F12">
-        <v>31197.40939018871</v>
-      </c>
-      <c r="G12">
         <v>30828.637761061971</v>
       </c>
     </row>
@@ -1366,13 +1296,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1395,7 +1325,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1418,7 +1348,7 @@
         <v>0.74559960301084749</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1441,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1464,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1487,7 +1417,7 @@
         <v>0.25440039698915251</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1510,7 +1440,7 @@
         <v>0.8538364409654523</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1533,7 +1463,7 @@
         <v>2.2319769441928702E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1556,7 +1486,7 @@
         <v>1.507841315333267E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1579,7 +1509,7 @@
         <v>0.10041324599182851</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1602,7 +1532,7 @@
         <v>1.70857131887975E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1625,7 +1555,7 @@
         <v>1.0342580180791731E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1659,9 +1589,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1681,7 +1611,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1701,7 +1631,7 @@
         <v>106995.39212639219</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Added an accounting for the possibility of an adductName column in the AccucorLoader.
Also restored that column in all the test files where it had been removed.

Files checked in: DataRepo/data/tests/accucor_with_multiple_labels/accucor.xlsx DataRepo/data/tests/accucor_with_multiple_labels/accucor_invalid_label.xlsx DataRepo/data/tests/data_submission/accucor1.xlsx DataRepo/data/tests/data_submission/accucor2.xlsx DataRepo/data/tests/small_obob/small_obob_maven_6eaas_inf_blank_sample.xlsx DataRepo/data/tests/small_obob/small_obob_maven_6eaas_inf_glucose.xlsx DataRepo/data/tests/small_obob/small_obob_maven_6eaas_inf_glucose_conflicting.xlsx DataRepo/loaders/base/converted_table_loader.py DataRepo/loaders/peak_annotations_loader.py outputFile.xlsx
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/accucor_with_multiple_labels/accucor.xlsx
+++ b/DataRepo/data/tests/accucor_with_multiple_labels/accucor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/data/tests/accucor_with_multiple_labels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-LOCAL/TRACEBASE/tracebase/DataRepo/data/tests/accucor_with_multiple_labels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5704C6-7D41-C94F-BAAB-E64B13FD9B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CA6893-911F-DD46-AAE4-EE4893A38ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="33">
   <si>
     <t>label</t>
   </si>
@@ -177,11 +177,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1041,33 +1042,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1075,19 +1079,22 @@
         <v>0</v>
       </c>
       <c r="C2">
+        <v>1.0402279999999999</v>
+      </c>
+      <c r="D2">
         <v>85750.89959084439</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>113767.0574420943</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>84190.488562416678</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>79775.721893427981</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1106,8 +1113,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1126,8 +1136,11 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1141,13 +1154,16 @@
         <v>0</v>
       </c>
       <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>19425.606829438329</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>27219.670232964221</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1155,19 +1171,22 @@
         <v>0</v>
       </c>
       <c r="C6">
+        <v>1.078981</v>
+      </c>
+      <c r="D6">
         <v>5591786.8355261376</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>4910135.5859680166</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>4380090.4658212066</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>4692672.7282388248</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1175,19 +1194,22 @@
         <v>1</v>
       </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>195595.3956708484</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>229303.59604486561</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>138481.27457236411</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>122669.1299826532</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1195,19 +1217,22 @@
         <v>2</v>
       </c>
       <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>112278.4380717509</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>154169.69247568949</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>83200.539628753497</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>82870.740571524482</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1215,19 +1240,22 @@
         <v>3</v>
       </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>137433.18004431319</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>197000.5904698009</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>590367.37452902028</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>551869.74742725445</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1235,19 +1263,22 @@
         <v>4</v>
       </c>
       <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
         <v>12741.57163112608</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>22989.486835416861</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>5529.4783128642057</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>9390.2832529520238</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1255,19 +1286,22 @@
         <v>5</v>
       </c>
       <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
         <v>2688.0625616373491</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>12430.02116063707</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>6595.5721957555343</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>5684.2671061387146</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1275,15 +1309,18 @@
         <v>6</v>
       </c>
       <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
         <v>800781.82886352425</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1155697.9116251131</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>31197.40939018871</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>30828.637761061971</v>
       </c>
     </row>

</xml_diff>